<commit_message>
Write teh thing, cause the Excel sheet seems to be corrput.
</commit_message>
<xml_diff>
--- a/SampleMatches.xlsx
+++ b/SampleMatches.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -66,11 +66,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,7 +376,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -404,16 +405,16 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>4290</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>7161</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>6209</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>9053</v>
       </c>
     </row>
@@ -421,16 +422,16 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>8683</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>8295</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>5815</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>4751</v>
       </c>
     </row>
@@ -438,16 +439,16 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>6504</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>8517</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>4718</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>6901</v>
       </c>
     </row>
@@ -456,16 +457,16 @@
         <f xml:space="preserve"> A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>6798</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>6299</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>8284</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>10862</v>
       </c>
     </row>
@@ -474,16 +475,16 @@
         <f t="shared" ref="A6:A30" si="0" xml:space="preserve"> A5+1</f>
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>10769</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>9278</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>3147</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>3708</v>
       </c>
     </row>
@@ -492,16 +493,16 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>4721</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>10997</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>9793</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>4720</v>
       </c>
     </row>
@@ -510,16 +511,16 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>5681</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>8424</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>5936</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>10994</v>
       </c>
     </row>
@@ -528,16 +529,16 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>5890</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>4291</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>3781</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>8214</v>
       </c>
     </row>
@@ -546,16 +547,16 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>8814</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>11000</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>6816</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>4549</v>
       </c>
     </row>
@@ -564,16 +565,16 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>4753</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>6041</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>7785</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>4723</v>
       </c>
     </row>

</xml_diff>